<commit_message>
polish and add commit
</commit_message>
<xml_diff>
--- a/signal table.xlsx
+++ b/signal table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ming_Loongson\Documents\lab\ucas18_19\mycpu_verify\rtl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ming_Loongson\Documents\lab\ucas18_19\mycpu_verify\rtl\myCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1549,9 +1549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix bugs, pass on FPGA board
</commit_message>
<xml_diff>
--- a/signal table.xlsx
+++ b/signal table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="349">
   <si>
     <t>op</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1203,6 +1203,80 @@
   </si>
   <si>
     <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExcCode_Int   5'h00</t>
+  </si>
+  <si>
+    <t>ExcCode_AdEL  5'h04</t>
+  </si>
+  <si>
+    <t>ExcCode_AdES  5'h05</t>
+  </si>
+  <si>
+    <t>ExcCode_Sys   5'h08</t>
+  </si>
+  <si>
+    <t>ExcCode_Bp    5'h09</t>
+  </si>
+  <si>
+    <t>ExcCode_RI    5'h0a</t>
+  </si>
+  <si>
+    <t>ExcCode_Ov    5'h0c</t>
+  </si>
+  <si>
+    <t>ExcCode_Ov</t>
+  </si>
+  <si>
+    <t>ExcCode_AdEL</t>
+  </si>
+  <si>
+    <t>ExcCode_AdES</t>
+  </si>
+  <si>
+    <t>inst_eret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_mfc0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_mtc0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_syscall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_break</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001101</t>
+  </si>
+  <si>
+    <t>001100</t>
+  </si>
+  <si>
+    <t>010000</t>
+  </si>
+  <si>
+    <t>rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00100</t>
+  </si>
+  <si>
+    <t>ExcCode_Sys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExcCode_Bp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1547,2059 +1621,2068 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9" style="2"/>
-    <col min="5" max="5" width="10.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1"/>
-    <col min="7" max="7" width="2.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9" style="1"/>
-    <col min="13" max="13" width="20.25" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="11.75" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.25" style="1" customWidth="1"/>
-    <col min="17" max="18" width="7.375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="22.75" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="1"/>
+    <col min="2" max="5" width="9" style="2"/>
+    <col min="6" max="6" width="10.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="1"/>
+    <col min="14" max="14" width="20.25" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="1"/>
+    <col min="16" max="16" width="11.75" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.25" style="1" customWidth="1"/>
+    <col min="18" max="19" width="7.375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="22.75" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>345</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K4" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K5" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S5" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K6" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q6" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q7" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K8" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K9" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K10" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q10" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K11" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q11" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K12" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K13" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T13" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K14" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K15" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="M16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q16" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S16" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K17" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q17" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S17" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K18" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q18" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S18" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K19" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q19" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="I20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K20" s="1" t="s">
-        <v>58</v>
+        <v>279</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="M20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="S21" s="1" t="s">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T21" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="H22" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K22" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q22" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="H23" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K23" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q23" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q24" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S24" s="1" t="s">
+      <c r="T24" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K25" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K26" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q26" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K27" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q27" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K28" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L28" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P28" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q28" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K29" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P29" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q29" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K30" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q30" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R30" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K31" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q31" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R31" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K32" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="S33" s="1" t="s">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T33" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K34" s="1" t="s">
-        <v>211</v>
+        <v>279</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>211</v>
       </c>
       <c r="M34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="R34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="T34" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K35" s="1" t="s">
-        <v>211</v>
+        <v>279</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>211</v>
       </c>
       <c r="M35" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="N35" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K36" s="1" t="s">
-        <v>211</v>
+        <v>279</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>211</v>
       </c>
       <c r="M36" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K37" s="1" t="s">
-        <v>211</v>
+        <v>279</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>211</v>
       </c>
       <c r="M37" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="P37" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="R37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="T37" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K38" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="P38" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="P38" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q38" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T38" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K39" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="P39" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q39" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S39" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T39" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>162</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K40" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="P40" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q40" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S40" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T40" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K41" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="O41" s="1" t="s">
+      <c r="P41" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="P41" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q41" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S41" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T41" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="S42" s="1" t="s">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T42" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>237</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>96</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>279</v>
+        <v>96</v>
       </c>
       <c r="K43" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O43" s="1" t="s">
+      <c r="P43" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="P43" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q43" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="U43" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>239</v>
       </c>
@@ -3609,144 +3692,144 @@
       <c r="D44" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="I44" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K44" s="1" t="s">
-        <v>222</v>
+        <v>279</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>222</v>
       </c>
       <c r="M44" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N44" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="O44" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="P44" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q44" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S44" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T44" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="T44" s="1" t="s">
+      <c r="U44" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>248</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>96</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>279</v>
+        <v>96</v>
       </c>
       <c r="K45" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="M45" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="N45" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="N45" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="O45" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S45" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T45" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>249</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="I46" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K46" s="1" t="s">
-        <v>201</v>
+        <v>279</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>201</v>
       </c>
       <c r="M46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="N46" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="N46" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="O46" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S46" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T46" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>250</v>
       </c>
@@ -3756,47 +3839,47 @@
       <c r="D47" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>96</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>279</v>
+        <v>96</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>201</v>
+        <v>279</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>201</v>
       </c>
       <c r="M47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="N47" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="N47" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="O47" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S47" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T47" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>251</v>
       </c>
@@ -3806,47 +3889,47 @@
       <c r="D48" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K48" s="1" t="s">
-        <v>201</v>
+        <v>279</v>
       </c>
       <c r="L48" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M48" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="N48" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="N48" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="O48" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S48" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T48" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>266</v>
       </c>
@@ -3856,552 +3939,651 @@
       <c r="D49" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K49" s="1" t="s">
-        <v>201</v>
+        <v>279</v>
       </c>
       <c r="L49" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M49" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="N49" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="N49" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="O49" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S49" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T49" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>252</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K50" s="1" t="s">
-        <v>201</v>
+        <v>279</v>
       </c>
       <c r="L50" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M50" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="N50" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="O50" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S50" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>284</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K51" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L51" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="L51" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="N51" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="N51" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="O51" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="P51" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="R51" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>285</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K52" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L52" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="M52" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="M52" s="1" t="s">
+      <c r="N52" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="N52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="O52" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="P52" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S52" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T52" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>286</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>276</v>
       </c>
       <c r="H53" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K53" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L53" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="M53" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="N53" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="N53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="O53" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="P53" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S53" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T53" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>287</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>276</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="J54" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K54" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="M54" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="M54" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="N54" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="O54" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="O54" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="P54" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S54" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T54" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>288</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K55" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="M55" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M55" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="N55" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="O55" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="O55" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="P55" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S55" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T55" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>289</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="J56" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="K56" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="L56" s="1" t="s">
+      <c r="M56" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M56" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="N56" s="1" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S56" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T56" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>290</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="K57" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>222</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="S57" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T57" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>291</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>276</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I58" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="M58" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="M58" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="N58" s="1" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>292</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="J59" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>222</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>293</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="I60" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>222</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>279</v>
+        <v>201</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>201</v>
+        <v>223</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="T65" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="T66" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T67" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T68" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T69" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T70" s="1" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bugs in CP0 clear ueseless code delete E stage forward
</commit_message>
<xml_diff>
--- a/signal table.xlsx
+++ b/signal table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="362">
   <si>
     <t>op</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1073,10 +1073,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1117,6 +1113,211 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>REG_FROM_HALF_S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG_FROM_BYTE_U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG_FROM_HALF_U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101000</t>
+  </si>
+  <si>
+    <t>101001</t>
+  </si>
+  <si>
+    <t>101010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101110 </t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExcCode_Int   5'h00</t>
+  </si>
+  <si>
+    <t>ExcCode_AdEL  5'h04</t>
+  </si>
+  <si>
+    <t>ExcCode_AdES  5'h05</t>
+  </si>
+  <si>
+    <t>ExcCode_Sys   5'h08</t>
+  </si>
+  <si>
+    <t>ExcCode_Bp    5'h09</t>
+  </si>
+  <si>
+    <t>ExcCode_RI    5'h0a</t>
+  </si>
+  <si>
+    <t>ExcCode_Ov    5'h0c</t>
+  </si>
+  <si>
+    <t>ExcCode_Ov</t>
+  </si>
+  <si>
+    <t>ExcCode_AdEL</t>
+  </si>
+  <si>
+    <t>ExcCode_AdES</t>
+  </si>
+  <si>
+    <t>inst_eret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_mfc0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_mtc0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_syscall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_break</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010000</t>
+  </si>
+  <si>
+    <t>rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00100</t>
+  </si>
+  <si>
+    <t>ExcCode_Sys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExcCode_Bp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`define BRANCH_IMM         2'b01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BRANCH_IMM</t>
+  </si>
+  <si>
+    <t>`define BRANCH_REG         2'b10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">BRANCH_REG </t>
+  </si>
+  <si>
+    <t>`define BRANCH_INDEX       2'b11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BRANCH_INDEX</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sig_exc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXC_ERET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXC_BRK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXC_SYS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXC_MFC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXC_MTC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>REG_FROM_JOIN_R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1125,208 +1326,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REG_FROM_HALF_S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG_FROM_BYTE_U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REG_FROM_HALF_U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101000</t>
-  </si>
-  <si>
-    <t>101001</t>
-  </si>
-  <si>
-    <t>101010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101110 </t>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExcCode_Int   5'h00</t>
-  </si>
-  <si>
-    <t>ExcCode_AdEL  5'h04</t>
-  </si>
-  <si>
-    <t>ExcCode_AdES  5'h05</t>
-  </si>
-  <si>
-    <t>ExcCode_Sys   5'h08</t>
-  </si>
-  <si>
-    <t>ExcCode_Bp    5'h09</t>
-  </si>
-  <si>
-    <t>ExcCode_RI    5'h0a</t>
-  </si>
-  <si>
-    <t>ExcCode_Ov    5'h0c</t>
-  </si>
-  <si>
-    <t>ExcCode_Ov</t>
-  </si>
-  <si>
-    <t>ExcCode_AdEL</t>
-  </si>
-  <si>
-    <t>ExcCode_AdES</t>
-  </si>
-  <si>
-    <t>inst_eret</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inst_mfc0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inst_mtc0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inst_syscall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inst_break</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010000</t>
-  </si>
-  <si>
-    <t>rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00100</t>
-  </si>
-  <si>
-    <t>ExcCode_Sys</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExcCode_Bp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>`define BRANCH_IMM         2'b01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BRANCH_IMM</t>
-  </si>
-  <si>
-    <t>`define BRANCH_REG         2'b10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">BRANCH_REG </t>
-  </si>
-  <si>
-    <t>`define BRANCH_INDEX       2'b11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BRANCH_INDEX</t>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sig_exc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXC_ERET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXC_BRK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXC_SYS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXC_MFC0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXC_MTC0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1711,9 +1715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1727,7 +1731,7 @@
     <col min="10" max="10" width="11.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="1"/>
     <col min="15" max="15" width="20.25" style="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="1"/>
@@ -1743,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>260</v>
@@ -1752,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>29</v>
@@ -1814,7 +1818,7 @@
         <v>77</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>210</v>
@@ -1917,7 +1921,7 @@
         <v>66</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>210</v>
@@ -2491,10 +2495,10 @@
         <v>66</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>210</v>
@@ -2503,7 +2507,7 @@
         <v>267</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>61</v>
@@ -2541,7 +2545,7 @@
         <v>66</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>95</v>
@@ -2585,7 +2589,7 @@
         <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>66</v>
@@ -2632,7 +2636,7 @@
         <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>66</v>
@@ -2679,7 +2683,7 @@
         <v>25</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>66</v>
@@ -2715,7 +2719,7 @@
         <v>197</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -2729,7 +2733,7 @@
         <v>27</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>66</v>
@@ -2765,12 +2769,12 @@
         <v>217</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="U21" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
@@ -2790,7 +2794,7 @@
         <v>180</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>209</v>
@@ -2840,10 +2844,10 @@
         <v>180</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>210</v>
@@ -2893,7 +2897,7 @@
         <v>183</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>209</v>
@@ -2926,7 +2930,7 @@
         <v>217</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
@@ -2943,7 +2947,7 @@
         <v>184</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>210</v>
@@ -2990,7 +2994,7 @@
         <v>68</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>210</v>
@@ -3037,7 +3041,7 @@
         <v>70</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>211</v>
@@ -3084,7 +3088,7 @@
         <v>72</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>211</v>
@@ -3131,7 +3135,7 @@
         <v>73</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>211</v>
@@ -3732,7 +3736,7 @@
         <v>254</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>66</v>
@@ -3785,7 +3789,7 @@
         <v>183</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>66</v>
@@ -3835,7 +3839,7 @@
         <v>252</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>264</v>
@@ -3882,7 +3886,7 @@
         <v>253</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>264</v>
@@ -3932,7 +3936,7 @@
         <v>263</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>264</v>
@@ -3982,7 +3986,7 @@
         <v>262</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>264</v>
@@ -4032,7 +4036,7 @@
         <v>261</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>264</v>
@@ -4082,7 +4086,7 @@
         <v>257</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>264</v>
@@ -4129,13 +4133,13 @@
         <v>282</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>264</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>210</v>
@@ -4144,13 +4148,13 @@
         <v>267</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>304</v>
+        <v>359</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>216</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>217</v>
@@ -4173,13 +4177,13 @@
         <v>283</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>264</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>210</v>
@@ -4188,13 +4192,13 @@
         <v>267</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>251</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P52" s="1" t="s">
         <v>217</v>
@@ -4226,10 +4230,10 @@
         <v>264</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>210</v>
@@ -4238,13 +4242,13 @@
         <v>267</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>216</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>217</v>
@@ -4276,10 +4280,10 @@
         <v>264</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>210</v>
@@ -4288,16 +4292,16 @@
         <v>267</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>218</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>267</v>
@@ -4326,7 +4330,7 @@
         <v>264</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>210</v>
@@ -4335,7 +4339,7 @@
         <v>267</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>216</v>
@@ -4373,7 +4377,7 @@
         <v>264</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>210</v>
@@ -4382,7 +4386,7 @@
         <v>267</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>303</v>
+        <v>358</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>216</v>
@@ -4411,7 +4415,7 @@
         <v>278</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>52</v>
@@ -4420,7 +4424,7 @@
         <v>264</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>210</v>
@@ -4458,7 +4462,7 @@
         <v>279</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>52</v>
@@ -4467,10 +4471,10 @@
         <v>264</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>210</v>
@@ -4482,7 +4486,7 @@
         <v>217</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="O58" s="1" t="s">
         <v>218</v>
@@ -4505,7 +4509,7 @@
         <v>280</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>52</v>
@@ -4514,13 +4518,13 @@
         <v>264</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>210</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>292</v>
+        <v>360</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>217</v>
@@ -4549,7 +4553,7 @@
         <v>281</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>52</v>
@@ -4564,7 +4568,7 @@
         <v>210</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>292</v>
+        <v>361</v>
       </c>
       <c r="M60" s="1" t="s">
         <v>217</v>
@@ -4590,25 +4594,25 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>264</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>267</v>
@@ -4617,10 +4621,10 @@
         <v>57</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="P62" s="1" t="s">
         <v>57</v>
@@ -4637,16 +4641,16 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>264</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>52</v>
@@ -4655,7 +4659,7 @@
         <v>264</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>212</v>
@@ -4664,16 +4668,16 @@
         <v>267</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="Q63" s="1" t="s">
         <v>267</v>
@@ -4687,16 +4691,16 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>330</v>
-      </c>
       <c r="C64" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>52</v>
@@ -4705,7 +4709,7 @@
         <v>264</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>212</v>
@@ -4714,16 +4718,16 @@
         <v>267</v>
       </c>
       <c r="M64" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P64" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="N64" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="O64" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="P64" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="Q64" s="1" t="s">
         <v>267</v>
@@ -4735,33 +4739,33 @@
         <v>197</v>
       </c>
       <c r="U64" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>256</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>264</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>267</v>
@@ -4770,10 +4774,10 @@
         <v>57</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="P65" s="1" t="s">
         <v>57</v>
@@ -4788,33 +4792,33 @@
         <v>197</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>256</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>264</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>267</v>
@@ -4823,10 +4827,10 @@
         <v>57</v>
       </c>
       <c r="N66" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="O66" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="O66" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="P66" s="1" t="s">
         <v>57</v>
@@ -4841,27 +4845,27 @@
         <v>197</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="U67" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="U68" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="U69" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="U70" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>